<commit_message>
Histogram of RC chasings
</commit_message>
<xml_diff>
--- a/data/reduced_data.xlsx
+++ b/data/reduced_data.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20406"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20407"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Agarwal Lab\Corentin\Python\clusterGUI\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{399D3AD5-7A65-4499-8908-C4106A2AA7B0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FABAAAC4-46B0-418D-A504-A1B6C166E3B0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11625" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
@@ -281,7 +281,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -303,6 +303,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -335,7 +341,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -351,6 +357,8 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -667,8 +675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AS100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AG24" sqref="AG24"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1394,140 +1402,140 @@
         <v>-1.3168224775611159</v>
       </c>
     </row>
-    <row r="6" spans="1:45" s="3" customFormat="1">
-      <c r="A6" s="2" t="s">
+    <row r="6" spans="1:45" s="16" customFormat="1">
+      <c r="A6" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="16">
         <v>23</v>
       </c>
-      <c r="C6" s="3">
-        <v>1</v>
-      </c>
-      <c r="D6" s="3">
-        <v>1</v>
-      </c>
-      <c r="E6" s="3">
+      <c r="C6" s="16">
+        <v>1</v>
+      </c>
+      <c r="D6" s="16">
+        <v>1</v>
+      </c>
+      <c r="E6" s="16">
         <v>10</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="16">
         <v>57</v>
       </c>
-      <c r="G6" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="H6" s="3">
+      <c r="G6" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="H6" s="16">
         <v>32.71</v>
       </c>
-      <c r="I6" s="3">
+      <c r="I6" s="16">
         <v>33.979999999999997</v>
       </c>
-      <c r="J6" s="3">
+      <c r="J6" s="16">
         <v>1.269999999999996</v>
       </c>
-      <c r="K6" s="3">
+      <c r="K6" s="16">
         <v>2</v>
       </c>
-      <c r="L6" s="3">
+      <c r="L6" s="16">
         <v>17.666666666666668</v>
       </c>
-      <c r="M6" s="3">
+      <c r="M6" s="16">
         <v>2</v>
       </c>
-      <c r="N6" s="3">
+      <c r="N6" s="16">
         <v>7.8630644717601257</v>
       </c>
-      <c r="O6" s="3">
+      <c r="O6" s="16">
         <v>2.1365103789854469</v>
       </c>
-      <c r="P6" s="3">
+      <c r="P6" s="16">
         <v>1.0693175088061515</v>
       </c>
-      <c r="Q6" s="3">
+      <c r="Q6" s="16">
         <v>0.71989909100637894</v>
       </c>
-      <c r="R6" s="3">
+      <c r="R6" s="16">
         <v>0.3</v>
       </c>
-      <c r="S6" s="3">
+      <c r="S6" s="16">
         <v>1.3333333333333335</v>
       </c>
-      <c r="T6" s="3">
+      <c r="T6" s="16">
         <v>1.1666666666666667</v>
       </c>
-      <c r="U6" s="3">
+      <c r="U6" s="16">
         <v>-1.9259502618856044</v>
       </c>
-      <c r="V6" s="3">
+      <c r="V6" s="16">
         <v>0.12583495182967788</v>
       </c>
-      <c r="W6" s="3">
+      <c r="W6" s="16">
         <v>-1.6208335462396188</v>
       </c>
-      <c r="X6" s="3">
+      <c r="X6" s="16">
         <v>0.24502285955661873</v>
       </c>
-      <c r="Y6" s="3">
+      <c r="Y6" s="16">
         <v>2.2932327225291642</v>
       </c>
-      <c r="Z6" s="3">
+      <c r="Z6" s="16">
         <v>3.2069135079441851</v>
       </c>
-      <c r="AA6" s="3">
+      <c r="AA6" s="16">
         <v>0.14553169018086567</v>
       </c>
-      <c r="AB6" s="3">
+      <c r="AB6" s="16">
         <v>3.1351162252380163</v>
       </c>
-      <c r="AC6" s="3">
+      <c r="AC6" s="16">
         <v>-7.6767386630186132E-2</v>
       </c>
-      <c r="AD6" s="3">
+      <c r="AD6" s="16">
         <v>-2.0031400658951291</v>
       </c>
-      <c r="AE6" s="3">
+      <c r="AE6" s="16">
         <v>-1.5572881454785688</v>
       </c>
-      <c r="AF6" s="3">
+      <c r="AF6" s="16">
         <v>0.85088390816787152</v>
       </c>
-      <c r="AG6" s="3">
+      <c r="AG6" s="16">
         <v>1.3000577375420503</v>
       </c>
-      <c r="AH6" s="5">
+      <c r="AH6" s="16">
         <v>9067.1200000000008</v>
       </c>
-      <c r="AI6" s="3">
+      <c r="AI6" s="16">
         <v>1.4647634137417116</v>
       </c>
-      <c r="AJ6" s="3">
+      <c r="AJ6" s="16">
         <v>9.1151079700916932E-2</v>
       </c>
-      <c r="AK6" s="3">
+      <c r="AK6" s="16">
         <v>6.6747145001146695</v>
       </c>
-      <c r="AL6" s="3">
+      <c r="AL6" s="16">
         <v>-0.85221746461946424</v>
       </c>
-      <c r="AM6" s="3">
+      <c r="AM6" s="16">
         <v>2.8008645281667941</v>
       </c>
-      <c r="AN6" s="3">
+      <c r="AN6" s="16">
         <v>-0.9886930046359419</v>
       </c>
-      <c r="AO6" s="3">
+      <c r="AO6" s="16">
         <v>-0.83679947404251165</v>
       </c>
-      <c r="AP6" s="3">
+      <c r="AP6" s="16">
         <v>-0.52164648072605835</v>
       </c>
-      <c r="AQ6" s="3">
+      <c r="AQ6" s="16">
         <v>0.25226370315421665</v>
       </c>
-      <c r="AR6" s="3">
+      <c r="AR6" s="16">
         <v>-0.97839146736168869</v>
       </c>
-      <c r="AS6" s="3">
+      <c r="AS6" s="16">
         <v>-0.52028715878154586</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Critical bug in the order (or ranking) by chasing and approaches.
I was using the np.argsort function, which does not return the order but the indices that would be necessary to sort. So to get the order of an array, one needs to use list(array).index(idx)!! This drastically changed the results for the approach order of the rich club.
</commit_message>
<xml_diff>
--- a/data/reduced_data.xlsx
+++ b/data/reduced_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20416"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Agarwal Lab\Corentin\Python\NoSeMaze\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B96E64C6-362E-4DEE-8C85-8A17BF70FF6A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ADA8910-CD3A-40C2-B146-7ABD82BEC999}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11625" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,15 +22,7 @@
     <definedName name="_xlchart.v1.11" hidden="1">Sheet1!$AV$2:$AV$100</definedName>
     <definedName name="_xlchart.v1.12" hidden="1">Sheet1!$AW$1</definedName>
     <definedName name="_xlchart.v1.13" hidden="1">Sheet1!$AW$2:$AW$100</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">Sheet1!$AX$1</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">Sheet1!$AX$2:$AX$100</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">Sheet1!$AU$1</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">Sheet1!$AU$2:$AU$100</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">Sheet1!$AV$1</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">Sheet1!$AV$2:$AV$100</definedName>
     <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$AV$1</definedName>
-    <definedName name="_xlchart.v1.20" hidden="1">Sheet1!$AW$1</definedName>
-    <definedName name="_xlchart.v1.21" hidden="1">Sheet1!$AW$2:$AW$100</definedName>
     <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$AV$2:$AV$100</definedName>
     <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$AW$1</definedName>
     <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$AW$2:$AW$100</definedName>
@@ -44,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="88">
   <si>
     <t>Mouse_RFID</t>
   </si>
@@ -306,6 +298,9 @@
   <si>
     <t>All</t>
   </si>
+  <si>
+    <t>RC values</t>
+  </si>
 </sst>
 </file>
 
@@ -475,17 +470,17 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.17</cx:f>
+        <cx:f>_xlchart.v1.9</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.19</cx:f>
+        <cx:f>_xlchart.v1.11</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="2">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.21</cx:f>
+        <cx:f>_xlchart.v1.13</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -523,8 +518,8 @@
         <cx:series layoutId="boxWhisker" uniqueId="{CF481420-33C5-4BEB-93CA-53BFE9ACEE07}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.16</cx:f>
-              <cx:v>RC</cx:v>
+              <cx:f>_xlchart.v1.8</cx:f>
+              <cx:v>RC values</cx:v>
             </cx:txData>
           </cx:tx>
           <cx:dataId val="0"/>
@@ -536,7 +531,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{70BCDA28-DBA0-4C96-B679-1D17C29C18CD}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.18</cx:f>
+              <cx:f>_xlchart.v1.10</cx:f>
               <cx:v>Mutants</cx:v>
             </cx:txData>
           </cx:tx>
@@ -549,7 +544,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{EA777DA6-40F3-451D-B349-E64FA6013D70}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.20</cx:f>
+              <cx:f>_xlchart.v1.12</cx:f>
               <cx:v>Others</cx:v>
             </cx:txData>
           </cx:tx>
@@ -631,22 +626,22 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.9</cx:f>
+        <cx:f>_xlchart.v1.1</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.11</cx:f>
+        <cx:f>_xlchart.v1.3</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="2">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.13</cx:f>
+        <cx:f>_xlchart.v1.5</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="3">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.15</cx:f>
+        <cx:f>_xlchart.v1.7</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -656,8 +651,8 @@
         <cx:series layoutId="boxWhisker" uniqueId="{BF8E49F0-D2BB-4AC9-AC59-3EC6F979FBC8}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.8</cx:f>
-              <cx:v>RC</cx:v>
+              <cx:f>_xlchart.v1.0</cx:f>
+              <cx:v>RC values</cx:v>
             </cx:txData>
           </cx:tx>
           <cx:dataId val="0"/>
@@ -669,7 +664,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{387E8E70-4CBD-4B03-83A9-4BC6ADEF90F4}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.10</cx:f>
+              <cx:f>_xlchart.v1.2</cx:f>
               <cx:v>Mutants</cx:v>
             </cx:txData>
           </cx:tx>
@@ -682,7 +677,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{CE993892-6F5A-4607-815A-55A279CCC0B5}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.12</cx:f>
+              <cx:f>_xlchart.v1.4</cx:f>
               <cx:v>Others</cx:v>
             </cx:txData>
           </cx:tx>
@@ -695,7 +690,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{F51E9B6B-2EF6-40EE-BA0B-6F9B5854C7C5}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.14</cx:f>
+              <cx:f>_xlchart.v1.6</cx:f>
               <cx:v>All</cx:v>
             </cx:txData>
           </cx:tx>
@@ -1942,16 +1937,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>51</xdr:col>
-      <xdr:colOff>79601</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>21090</xdr:rowOff>
+      <xdr:col>52</xdr:col>
+      <xdr:colOff>517751</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>144915</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>58</xdr:col>
-      <xdr:colOff>354465</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>78241</xdr:rowOff>
+      <xdr:col>60</xdr:col>
+      <xdr:colOff>183015</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>11566</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
@@ -1987,7 +1982,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="58972676" y="4259715"/>
+              <a:off x="60020426" y="3993015"/>
               <a:ext cx="4542064" cy="2743201"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -2320,8 +2315,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AX100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AP4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BC19" sqref="BC19"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O86" sqref="O86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2502,8 +2497,11 @@
       <c r="AS1" s="1" t="s">
         <v>82</v>
       </c>
+      <c r="AT1" s="23" t="s">
+        <v>83</v>
+      </c>
       <c r="AU1" s="32" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="AV1" s="33" t="s">
         <v>84</v>
@@ -2650,6 +2648,9 @@
       </c>
       <c r="AS2">
         <v>0.34948246529047805</v>
+      </c>
+      <c r="AT2" t="b">
+        <v>0</v>
       </c>
       <c r="AU2" s="26">
         <v>8459.2377777777783</v>
@@ -2800,6 +2801,9 @@
       <c r="AS3">
         <v>1.5468236302370428</v>
       </c>
+      <c r="AT3" t="b">
+        <v>0</v>
+      </c>
       <c r="AU3" s="26">
         <v>16292.339999999995</v>
       </c>
@@ -2949,6 +2953,9 @@
       <c r="AS4">
         <v>-0.40827656418750669</v>
       </c>
+      <c r="AT4" t="b">
+        <v>0</v>
+      </c>
       <c r="AU4" s="26">
         <v>6761.722222222219</v>
       </c>
@@ -3098,6 +3105,9 @@
       <c r="AS5">
         <v>-1.3168224775611159</v>
       </c>
+      <c r="AT5" t="b">
+        <v>0</v>
+      </c>
       <c r="AU5" s="26">
         <v>5220.4022222222202</v>
       </c>
@@ -3247,6 +3257,9 @@
       <c r="AS6" s="16">
         <v>-0.52028715878154586</v>
       </c>
+      <c r="AT6" t="b">
+        <v>1</v>
+      </c>
       <c r="AU6" s="26">
         <v>13468.974358974352</v>
       </c>
@@ -3396,6 +3409,9 @@
       <c r="AS7" s="3">
         <v>-0.84186745867216695</v>
       </c>
+      <c r="AT7" t="b">
+        <v>1</v>
+      </c>
       <c r="AU7" s="26">
         <v>11803.271794871798</v>
       </c>
@@ -3545,6 +3561,9 @@
       <c r="AS8">
         <v>-0.83843962932386018</v>
       </c>
+      <c r="AT8" t="b">
+        <v>0</v>
+      </c>
       <c r="AU8" s="27">
         <v>10424.417948717957</v>
       </c>
@@ -3694,6 +3713,9 @@
       <c r="AS9" s="14">
         <v>-0.1025026531927859</v>
       </c>
+      <c r="AT9" t="b">
+        <v>0</v>
+      </c>
       <c r="AU9" s="26">
         <v>5363.1820512820514</v>
       </c>
@@ -3843,6 +3865,9 @@
       <c r="AS10">
         <v>1.683982158454314</v>
       </c>
+      <c r="AT10" t="b">
+        <v>0</v>
+      </c>
       <c r="AU10" s="26">
         <v>6550.6307692307728</v>
       </c>
@@ -3992,6 +4017,9 @@
       <c r="AS11" s="7">
         <v>-0.53416634287655096</v>
       </c>
+      <c r="AT11" t="b">
+        <v>0</v>
+      </c>
       <c r="AU11" s="26">
         <v>4716.5809523809512</v>
       </c>
@@ -4141,6 +4169,9 @@
       <c r="AS12" s="3">
         <v>2.0552231043316693</v>
       </c>
+      <c r="AT12" t="b">
+        <v>1</v>
+      </c>
       <c r="AU12" s="28">
         <v>7560.2595238095246</v>
       </c>
@@ -4290,6 +4321,9 @@
       <c r="AS13" s="14">
         <v>0.9667014755664155</v>
       </c>
+      <c r="AT13" t="b">
+        <v>0</v>
+      </c>
       <c r="AU13" s="26">
         <v>5040.5138888888887</v>
       </c>
@@ -4439,6 +4473,9 @@
       <c r="AS14" s="3">
         <v>-0.44788644212468565</v>
       </c>
+      <c r="AT14" t="b">
+        <v>1</v>
+      </c>
       <c r="AU14" s="26">
         <v>1654.2888888888881</v>
       </c>
@@ -4588,6 +4625,9 @@
       <c r="AS15" s="3">
         <v>-0.9754904143948252</v>
       </c>
+      <c r="AT15" t="b">
+        <v>1</v>
+      </c>
       <c r="AU15" s="26">
         <v>2557.9809523809527</v>
       </c>
@@ -4737,6 +4777,9 @@
       <c r="AS16">
         <v>-2.5318163406889607</v>
       </c>
+      <c r="AT16" t="b">
+        <v>0</v>
+      </c>
       <c r="AU16" s="26">
         <v>3109.9285714285716</v>
       </c>
@@ -4886,6 +4929,9 @@
       <c r="AS17">
         <v>-0.69254294620224599</v>
       </c>
+      <c r="AT17" t="b">
+        <v>0</v>
+      </c>
       <c r="AU17" s="26">
         <v>2836.9380952380939</v>
       </c>
@@ -5032,6 +5078,9 @@
       <c r="AS18">
         <v>-2.1806177213128044</v>
       </c>
+      <c r="AT18" t="b">
+        <v>0</v>
+      </c>
       <c r="AU18" s="26">
         <v>10464.924444444447</v>
       </c>
@@ -5178,6 +5227,9 @@
       <c r="AS19">
         <v>-0.42964906455375212</v>
       </c>
+      <c r="AT19" t="b">
+        <v>0</v>
+      </c>
       <c r="AU19" s="26">
         <v>6908.9555555555544</v>
       </c>
@@ -5324,6 +5376,9 @@
       <c r="AS20">
         <v>1.1292254059619942</v>
       </c>
+      <c r="AT20" t="b">
+        <v>0</v>
+      </c>
       <c r="AU20" s="26">
         <v>5345.7111111111117</v>
       </c>
@@ -5470,6 +5525,9 @@
       <c r="AS21" s="12">
         <v>-0.16584066964212993</v>
       </c>
+      <c r="AT21" t="b">
+        <v>0</v>
+      </c>
       <c r="AU21" s="26">
         <v>7097.1044444444442</v>
       </c>
@@ -5581,6 +5639,9 @@
       <c r="AG22">
         <v>-1.7121074454103868</v>
       </c>
+      <c r="AT22" t="b">
+        <v>0</v>
+      </c>
       <c r="AW22" s="29">
         <v>3598.3179487179505</v>
       </c>
@@ -5721,6 +5782,9 @@
       <c r="AS23">
         <v>1.5466140507312964</v>
       </c>
+      <c r="AT23" t="b">
+        <v>0</v>
+      </c>
       <c r="AW23" s="29">
         <v>4299.0230769230766</v>
       </c>
@@ -5864,6 +5928,9 @@
       <c r="AS24">
         <v>-1.3009329464230408E-2</v>
       </c>
+      <c r="AT24" t="b">
+        <v>0</v>
+      </c>
       <c r="AW24" s="29">
         <v>3005.4666666666667</v>
       </c>
@@ -6007,6 +6074,9 @@
       <c r="AS25" s="3">
         <v>8.878426731065539E-2</v>
       </c>
+      <c r="AT25" t="b">
+        <v>1</v>
+      </c>
       <c r="AU25" s="26"/>
       <c r="AV25" s="24"/>
       <c r="AW25" s="29">
@@ -6152,6 +6222,9 @@
       <c r="AS26" s="3">
         <v>-0.47635450245024213</v>
       </c>
+      <c r="AT26" t="b">
+        <v>1</v>
+      </c>
       <c r="AU26" s="26"/>
       <c r="AV26" s="24"/>
       <c r="AW26" s="29">
@@ -6261,6 +6334,9 @@
       <c r="AG27" s="14">
         <v>1.9520240499640036</v>
       </c>
+      <c r="AT27" t="b">
+        <v>0</v>
+      </c>
       <c r="AU27" s="26"/>
       <c r="AV27" s="24"/>
       <c r="AW27" s="29">
@@ -6403,6 +6479,9 @@
       <c r="AS28" s="14">
         <v>-0.85408735988100781</v>
       </c>
+      <c r="AT28" t="b">
+        <v>0</v>
+      </c>
       <c r="AU28" s="26"/>
       <c r="AV28" s="24"/>
       <c r="AW28" s="29">
@@ -6548,6 +6627,9 @@
       <c r="AS29">
         <v>-0.38047516046763663</v>
       </c>
+      <c r="AT29" t="b">
+        <v>0</v>
+      </c>
       <c r="AW29" s="29">
         <v>5214.5023809523818</v>
       </c>
@@ -6691,6 +6773,9 @@
       <c r="AS30">
         <v>-1.832495606181747</v>
       </c>
+      <c r="AT30" t="b">
+        <v>0</v>
+      </c>
       <c r="AW30" s="29">
         <v>6103.0928571428567</v>
       </c>
@@ -6834,6 +6919,9 @@
       <c r="AS31" s="10">
         <v>0.36820732001139567</v>
       </c>
+      <c r="AT31" t="b">
+        <v>1</v>
+      </c>
       <c r="AU31" s="27"/>
       <c r="AV31" s="25"/>
       <c r="AW31" s="29">
@@ -6979,6 +7067,9 @@
       <c r="AS32">
         <v>-0.4602472125773438</v>
       </c>
+      <c r="AT32" t="b">
+        <v>0</v>
+      </c>
       <c r="AW32" s="29">
         <v>103.64444444444443</v>
       </c>
@@ -7122,6 +7213,9 @@
       <c r="AS33" s="14">
         <v>1.0998529620778026</v>
       </c>
+      <c r="AT33" t="b">
+        <v>0</v>
+      </c>
       <c r="AU33" s="26"/>
       <c r="AV33" s="24"/>
       <c r="AW33" s="29">
@@ -7267,6 +7361,9 @@
       <c r="AS34" s="3">
         <v>-0.28974637402891923</v>
       </c>
+      <c r="AT34" t="b">
+        <v>1</v>
+      </c>
       <c r="AU34" s="26"/>
       <c r="AV34" s="24"/>
       <c r="AW34" s="29">
@@ -7412,6 +7509,9 @@
       <c r="AS35" s="3">
         <v>0.84116388945701237</v>
       </c>
+      <c r="AT35" t="b">
+        <v>1</v>
+      </c>
       <c r="AU35" s="26"/>
       <c r="AV35" s="24"/>
       <c r="AW35" s="29">
@@ -7557,6 +7657,9 @@
       <c r="AS36">
         <v>2.4213295006572375</v>
       </c>
+      <c r="AT36" t="b">
+        <v>0</v>
+      </c>
       <c r="AW36" s="30">
         <v>1295.5555555555554</v>
       </c>
@@ -7700,6 +7803,9 @@
       <c r="AS37">
         <v>2.3927825936011313</v>
       </c>
+      <c r="AT37" t="b">
+        <v>0</v>
+      </c>
       <c r="AW37" s="29">
         <v>2111.8904761904755</v>
       </c>
@@ -7843,6 +7949,9 @@
       <c r="AS38" s="38">
         <v>1.3690578250979659</v>
       </c>
+      <c r="AT38" t="b">
+        <v>0</v>
+      </c>
       <c r="AW38" s="38">
         <v>2194.071428571428</v>
       </c>
@@ -7986,6 +8095,9 @@
       <c r="AS39">
         <v>3.7644763729008273</v>
       </c>
+      <c r="AT39" t="b">
+        <v>0</v>
+      </c>
       <c r="AW39" s="29">
         <v>3316.6595238095251</v>
       </c>
@@ -8129,6 +8241,9 @@
       <c r="AS40">
         <v>2.6884802587229593</v>
       </c>
+      <c r="AT40" t="b">
+        <v>0</v>
+      </c>
       <c r="AW40" s="29">
         <v>1514.2714285714287</v>
       </c>
@@ -8272,6 +8387,9 @@
       <c r="AS41" s="12">
         <v>-3.8966810695426714E-2</v>
       </c>
+      <c r="AT41" t="b">
+        <v>0</v>
+      </c>
       <c r="AU41" s="27"/>
       <c r="AV41" s="25"/>
       <c r="AW41" s="29">
@@ -8417,6 +8535,9 @@
       <c r="AS42">
         <v>0.93645320018107092</v>
       </c>
+      <c r="AT42" t="b">
+        <v>0</v>
+      </c>
       <c r="AW42" s="29">
         <v>3469.1222222222223</v>
       </c>
@@ -8560,6 +8681,9 @@
       <c r="AS43">
         <v>-0.9850741442965758</v>
       </c>
+      <c r="AT43" t="b">
+        <v>0</v>
+      </c>
       <c r="AW43" s="29">
         <v>5640.94888888889</v>
       </c>
@@ -8703,6 +8827,9 @@
       <c r="AS44">
         <v>0.64150730179007787</v>
       </c>
+      <c r="AT44" t="b">
+        <v>0</v>
+      </c>
       <c r="AW44" s="29">
         <v>743.48444444444408</v>
       </c>
@@ -8845,6 +8972,9 @@
       </c>
       <c r="AS45" s="3">
         <v>-1.7775359248502711</v>
+      </c>
+      <c r="AT45" t="b">
+        <v>1</v>
       </c>
       <c r="AU45" s="26"/>
       <c r="AV45" s="24"/>
@@ -8989,6 +9119,9 @@
       <c r="AS46">
         <v>-7.8471239574960799E-2</v>
       </c>
+      <c r="AT46" t="b">
+        <v>0</v>
+      </c>
       <c r="AX46" s="5">
         <v>5581.4880952380945</v>
       </c>
@@ -9129,6 +9262,9 @@
       <c r="AS47" s="36">
         <v>-0.7176826165849074</v>
       </c>
+      <c r="AT47" t="b">
+        <v>0</v>
+      </c>
       <c r="AW47" s="37"/>
       <c r="AX47" s="36">
         <v>7560.2595238095246</v>
@@ -9270,6 +9406,9 @@
       <c r="AS48">
         <v>-1.3960209518734064</v>
       </c>
+      <c r="AT48" t="b">
+        <v>0</v>
+      </c>
       <c r="AX48" s="5">
         <v>4744.2023809523798</v>
       </c>
@@ -9410,6 +9549,9 @@
       <c r="AS49">
         <v>0.9762635434307072</v>
       </c>
+      <c r="AT49" t="b">
+        <v>0</v>
+      </c>
       <c r="AX49" s="5">
         <v>5214.5023809523818</v>
       </c>
@@ -9550,6 +9692,9 @@
       <c r="AS50">
         <v>0.14580691061534123</v>
       </c>
+      <c r="AT50" t="b">
+        <v>0</v>
+      </c>
       <c r="AX50" s="5">
         <v>6103.0928571428567</v>
       </c>
@@ -9689,6 +9834,9 @@
       </c>
       <c r="AS51" s="12">
         <v>-3.1226968601109926</v>
+      </c>
+      <c r="AT51" t="b">
+        <v>0</v>
       </c>
       <c r="AU51" s="27"/>
       <c r="AV51" s="25"/>
@@ -9833,6 +9981,9 @@
       <c r="AS52">
         <v>-5.6781626813899004</v>
       </c>
+      <c r="AT52" t="b">
+        <v>0</v>
+      </c>
       <c r="AX52" s="5">
         <v>249.09166666666661</v>
       </c>
@@ -9972,6 +10123,9 @@
       </c>
       <c r="AS53" s="3">
         <v>0.10723883756532922</v>
+      </c>
+      <c r="AT53" t="b">
+        <v>1</v>
       </c>
       <c r="AU53" s="26"/>
       <c r="AV53" s="24"/>
@@ -10116,6 +10270,9 @@
       <c r="AS54" s="14">
         <v>3.5262671468445119</v>
       </c>
+      <c r="AT54" t="b">
+        <v>0</v>
+      </c>
       <c r="AU54" s="26"/>
       <c r="AV54" s="24"/>
       <c r="AW54" s="31"/>
@@ -10259,6 +10416,9 @@
       <c r="AS55">
         <v>-3.4173949813885214</v>
       </c>
+      <c r="AT55" t="b">
+        <v>0</v>
+      </c>
       <c r="AX55" s="5">
         <v>103.64444444444443</v>
       </c>
@@ -10399,6 +10559,9 @@
       <c r="AS56">
         <v>-1.1165572573528868</v>
       </c>
+      <c r="AT56" t="b">
+        <v>0</v>
+      </c>
       <c r="AX56" s="5">
         <v>306.64722222222224</v>
       </c>
@@ -10539,6 +10702,9 @@
       <c r="AS57">
         <v>-0.33423823756240972</v>
       </c>
+      <c r="AT57" t="b">
+        <v>0</v>
+      </c>
       <c r="AX57" s="5">
         <v>2521.9555555555553</v>
       </c>
@@ -10678,6 +10844,9 @@
       </c>
       <c r="AS58" s="14">
         <v>1.2774778727675618</v>
+      </c>
+      <c r="AT58" t="b">
+        <v>0</v>
       </c>
       <c r="AU58" s="26"/>
       <c r="AV58" s="24"/>
@@ -10822,6 +10991,9 @@
       <c r="AS59" s="3">
         <v>-2.378598969961113</v>
       </c>
+      <c r="AT59" t="b">
+        <v>1</v>
+      </c>
       <c r="AU59" s="26"/>
       <c r="AV59" s="24"/>
       <c r="AW59" s="31"/>
@@ -10965,6 +11137,9 @@
       <c r="AS60">
         <v>-1.5271317091886794</v>
       </c>
+      <c r="AT60" t="b">
+        <v>0</v>
+      </c>
       <c r="AX60" s="5">
         <v>1129.1305555555552</v>
       </c>
@@ -11104,6 +11279,9 @@
       </c>
       <c r="AS61" s="7">
         <v>-0.28257843674281974</v>
+      </c>
+      <c r="AT61" t="b">
+        <v>0</v>
       </c>
       <c r="AU61" s="27"/>
       <c r="AV61" s="25"/>
@@ -11248,6 +11426,9 @@
       <c r="AS62">
         <v>1.8007747279807815</v>
       </c>
+      <c r="AT62" t="b">
+        <v>0</v>
+      </c>
       <c r="AX62" s="5">
         <v>2111.8904761904755</v>
       </c>
@@ -11388,6 +11569,9 @@
       <c r="AS63">
         <v>1.5695172950748446</v>
       </c>
+      <c r="AT63" t="b">
+        <v>0</v>
+      </c>
       <c r="AX63" s="5">
         <v>2194.071428571428</v>
       </c>
@@ -11528,6 +11712,9 @@
       <c r="AS64">
         <v>0.75593869364718802</v>
       </c>
+      <c r="AT64" t="b">
+        <v>0</v>
+      </c>
       <c r="AX64" s="5">
         <v>3316.6595238095251</v>
       </c>
@@ -11667,6 +11854,9 @@
       </c>
       <c r="AS65" s="14">
         <v>-2.0867608939811682</v>
+      </c>
+      <c r="AT65" t="b">
+        <v>0</v>
       </c>
       <c r="AU65" s="26"/>
       <c r="AV65" s="24"/>
@@ -11811,6 +12001,9 @@
       <c r="AS66" s="14">
         <v>4.0065984348087227</v>
       </c>
+      <c r="AT66" t="b">
+        <v>0</v>
+      </c>
       <c r="AU66" s="26"/>
       <c r="AV66" s="24"/>
       <c r="AW66" s="31"/>
@@ -11954,6 +12147,9 @@
       <c r="AS67" s="3">
         <v>-2.3259443875727803</v>
       </c>
+      <c r="AT67" t="b">
+        <v>1</v>
+      </c>
       <c r="AU67" s="26"/>
       <c r="AV67" s="24"/>
       <c r="AW67" s="31"/>
@@ -12097,6 +12293,9 @@
       <c r="AS68">
         <v>0.17834989861328551</v>
       </c>
+      <c r="AT68" t="b">
+        <v>0</v>
+      </c>
       <c r="AX68" s="5">
         <v>1514.2714285714287</v>
       </c>
@@ -12236,6 +12435,9 @@
       </c>
       <c r="AS69" s="3">
         <v>-1.2703905026003313</v>
+      </c>
+      <c r="AT69" t="b">
+        <v>1</v>
       </c>
       <c r="AU69" s="26"/>
       <c r="AV69" s="24"/>
@@ -12380,6 +12582,9 @@
       <c r="AS70" s="3">
         <v>-1.1819566350730759</v>
       </c>
+      <c r="AT70" t="b">
+        <v>1</v>
+      </c>
       <c r="AU70" s="26"/>
       <c r="AV70" s="24"/>
       <c r="AW70" s="31"/>
@@ -12523,6 +12728,9 @@
       <c r="AS71">
         <v>-0.57468699327680639</v>
       </c>
+      <c r="AT71" t="b">
+        <v>0</v>
+      </c>
       <c r="AX71" s="5">
         <v>1078.5071428571434</v>
       </c>
@@ -12663,6 +12871,9 @@
       <c r="AS72">
         <v>2.2926386819995743</v>
       </c>
+      <c r="AT72" t="b">
+        <v>0</v>
+      </c>
       <c r="AX72" s="5">
         <v>3469.1222222222223</v>
       </c>
@@ -12802,6 +13013,9 @@
       </c>
       <c r="AS73" s="14">
         <v>-0.77699151457384019</v>
+      </c>
+      <c r="AT73" t="b">
+        <v>0</v>
       </c>
       <c r="AU73" s="26"/>
       <c r="AV73" s="24"/>
@@ -12946,6 +13160,9 @@
       <c r="AS74">
         <v>0.72494861681445966</v>
       </c>
+      <c r="AT74" t="b">
+        <v>0</v>
+      </c>
       <c r="AX74" s="5">
         <v>5640.94888888889</v>
       </c>
@@ -13085,6 +13302,9 @@
       </c>
       <c r="AS75" s="14">
         <v>8.8543920985754976E-2</v>
+      </c>
+      <c r="AT75" t="b">
+        <v>0</v>
       </c>
       <c r="AU75" s="26"/>
       <c r="AV75" s="24"/>
@@ -13229,6 +13449,9 @@
       <c r="AS76" s="3">
         <v>0.82605563398743442</v>
       </c>
+      <c r="AT76" t="b">
+        <v>1</v>
+      </c>
       <c r="AU76" s="26"/>
       <c r="AV76" s="24"/>
       <c r="AW76" s="31"/>
@@ -13372,6 +13595,9 @@
       <c r="AS77">
         <v>0.30800568287283636</v>
       </c>
+      <c r="AT77" t="b">
+        <v>0</v>
+      </c>
       <c r="AX77" s="5">
         <v>743.48444444444408</v>
       </c>
@@ -13511,6 +13737,9 @@
       </c>
       <c r="AS78" s="3">
         <v>0.14756766189504764</v>
+      </c>
+      <c r="AT78" t="b">
+        <v>1</v>
       </c>
       <c r="AU78" s="26"/>
       <c r="AV78" s="24"/>
@@ -13655,6 +13884,9 @@
       <c r="AS79">
         <v>-1.2059324788757626</v>
       </c>
+      <c r="AT79" t="b">
+        <v>0</v>
+      </c>
       <c r="AX79" s="5">
         <v>6514.5688888888881</v>
       </c>
@@ -13795,6 +14027,9 @@
       <c r="AS80">
         <v>3.2461244176412865</v>
       </c>
+      <c r="AT80" t="b">
+        <v>0</v>
+      </c>
       <c r="AX80" s="5">
         <v>6749.2688888888861</v>
       </c>
@@ -13935,6 +14170,9 @@
       <c r="AS81">
         <v>1.2729098049318985</v>
       </c>
+      <c r="AT81" t="b">
+        <v>0</v>
+      </c>
       <c r="AX81" s="5">
         <v>3767.9377777777781</v>
       </c>
@@ -14075,6 +14313,9 @@
       <c r="AS82">
         <v>-0.69196880090672275</v>
       </c>
+      <c r="AT82" t="b">
+        <v>0</v>
+      </c>
       <c r="AX82" s="5">
         <v>7582.620512820512</v>
       </c>
@@ -14176,6 +14417,9 @@
       <c r="AG83">
         <v>-0.37363724284975047</v>
       </c>
+      <c r="AT83" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="84" spans="1:50">
       <c r="A84" s="1" t="s">
@@ -14277,6 +14521,9 @@
       <c r="AG84">
         <v>0.40120303491222697</v>
       </c>
+      <c r="AT84" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="85" spans="1:50">
       <c r="A85" s="1" t="s">
@@ -14414,6 +14661,9 @@
       <c r="AS85">
         <v>1.4460932884609252</v>
       </c>
+      <c r="AT85" t="b">
+        <v>0</v>
+      </c>
       <c r="AX85" s="5">
         <v>3717.9487179487178</v>
       </c>
@@ -14554,6 +14804,9 @@
       <c r="AS86">
         <v>3.2534535185456801</v>
       </c>
+      <c r="AT86" t="b">
+        <v>0</v>
+      </c>
       <c r="AX86" s="5">
         <v>2574.3435897435897</v>
       </c>
@@ -14694,6 +14947,9 @@
       <c r="AS87">
         <v>0.76093525531259421</v>
       </c>
+      <c r="AT87" t="b">
+        <v>0</v>
+      </c>
       <c r="AX87" s="5">
         <v>1832.3538461538458</v>
       </c>
@@ -14798,6 +15054,9 @@
       <c r="AG88">
         <v>-1.1536045388779401</v>
       </c>
+      <c r="AT88" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="89" spans="1:50">
       <c r="A89" s="1" t="s">
@@ -14899,6 +15158,9 @@
       <c r="AG89">
         <v>0.23969354347864913</v>
       </c>
+      <c r="AT89" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="90" spans="1:50">
       <c r="A90" s="1" t="s">
@@ -15000,6 +15262,9 @@
       <c r="AG90">
         <v>1.3957687322087775</v>
       </c>
+      <c r="AT90" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="91" spans="1:50">
       <c r="A91" s="1" t="s">
@@ -15137,6 +15402,9 @@
       <c r="AS91">
         <v>4.5339478260516798E-2</v>
       </c>
+      <c r="AT91" t="b">
+        <v>0</v>
+      </c>
       <c r="AX91" s="5">
         <v>6076.3844444444439</v>
       </c>
@@ -15276,6 +15544,9 @@
       </c>
       <c r="AS92" s="14">
         <v>0.85986487523471289</v>
+      </c>
+      <c r="AT92" t="b">
+        <v>0</v>
       </c>
       <c r="AU92" s="26"/>
       <c r="AV92" s="24"/>
@@ -15420,6 +15691,9 @@
       <c r="AS93">
         <v>0.26259528395814308</v>
       </c>
+      <c r="AT93" t="b">
+        <v>0</v>
+      </c>
       <c r="AX93" s="5">
         <v>3973.068888888889</v>
       </c>
@@ -15559,6 +15833,9 @@
       </c>
       <c r="AS94" s="14">
         <v>-3.4183944834869502</v>
+      </c>
+      <c r="AT94" t="b">
+        <v>0</v>
       </c>
       <c r="AU94" s="26"/>
       <c r="AV94" s="24"/>
@@ -15703,6 +15980,9 @@
       <c r="AS95" s="3">
         <v>0.26095554216269767</v>
       </c>
+      <c r="AT95" t="b">
+        <v>1</v>
+      </c>
       <c r="AU95" s="26"/>
       <c r="AV95" s="24"/>
       <c r="AW95" s="31"/>
@@ -15846,6 +16126,9 @@
       <c r="AS96">
         <v>-0.13094442449868557</v>
       </c>
+      <c r="AT96" t="b">
+        <v>0</v>
+      </c>
       <c r="AX96" s="5">
         <v>3618.3355555555554</v>
       </c>
@@ -15985,6 +16268,9 @@
       </c>
       <c r="AS97" s="19">
         <v>0.89144268955263239</v>
+      </c>
+      <c r="AT97" t="b">
+        <v>0</v>
       </c>
       <c r="AU97" s="26"/>
       <c r="AV97" s="24"/>
@@ -16129,6 +16415,9 @@
       <c r="AS98" s="3">
         <v>-0.46992908504836128</v>
       </c>
+      <c r="AT98" t="b">
+        <v>1</v>
+      </c>
       <c r="AU98" s="26"/>
       <c r="AV98" s="24"/>
       <c r="AW98" s="31"/>
@@ -16272,6 +16561,9 @@
       <c r="AS99">
         <v>-0.78909983358457769</v>
       </c>
+      <c r="AT99" t="b">
+        <v>0</v>
+      </c>
       <c r="AX99" s="5">
         <v>4696.4955555555534</v>
       </c>
@@ -16411,6 +16703,9 @@
       </c>
       <c r="AS100">
         <v>0.69785175146133638</v>
+      </c>
+      <c r="AT100" t="b">
+        <v>0</v>
       </c>
       <c r="AX100" s="5">
         <v>6233.0088888888868</v>

</xml_diff>